<commit_message>
INTERFACE USUARIO E CRUD
</commit_message>
<xml_diff>
--- a/usuarios.xlsx
+++ b/usuarios.xlsx
@@ -12,12 +12,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>CPF</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Telefone</t>
+  </si>
+  <si>
+    <t>Endereço</t>
+  </si>
   <si>
     <t>Renan</t>
   </si>
   <si>
-    <t>123213213</t>
+    <t>1232131</t>
+  </si>
+  <si>
+    <t>renancewa@</t>
+  </si>
+  <si>
+    <t>231321321</t>
+  </si>
+  <si>
+    <t>dwadmwaniwadwa</t>
+  </si>
+  <si>
+    <t>dwad</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>213</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>d23213</t>
+  </si>
+  <si>
+    <t>dkwdmwa</t>
+  </si>
+  <si>
+    <t>31312</t>
+  </si>
+  <si>
+    <t>dwada</t>
+  </si>
+  <si>
+    <t>d213</t>
+  </si>
+  <si>
+    <t>21321</t>
   </si>
 </sst>
 </file>
@@ -62,18 +116,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:B2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Subindo projeto para a branch mainLuiz
</commit_message>
<xml_diff>
--- a/usuarios.xlsx
+++ b/usuarios.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="78">
   <si>
     <t>Nome</t>
   </si>
@@ -123,6 +123,129 @@
   </si>
   <si>
     <t>2321</t>
+  </si>
+  <si>
+    <t>Luiz</t>
+  </si>
+  <si>
+    <t>123123</t>
+  </si>
+  <si>
+    <t>luiz.antoniodesouza@gmaio.com</t>
+  </si>
+  <si>
+    <t>99034424</t>
+  </si>
+  <si>
+    <t>BarbaraHeliodora438</t>
+  </si>
+  <si>
+    <t>Luiz Antônio de Souza</t>
+  </si>
+  <si>
+    <t>luiz.antoniodesouza004@gmail.com</t>
+  </si>
+  <si>
+    <t>(35) 997344797</t>
+  </si>
+  <si>
+    <t>Rua Barbara Heliodora, 438</t>
+  </si>
+  <si>
+    <t>408.391.907-32</t>
+  </si>
+  <si>
+    <t>luiz.santos98@gmail.com</t>
+  </si>
+  <si>
+    <t>(11) 95234-6781</t>
+  </si>
+  <si>
+    <t>Rua das Flores, 123, Bairro Jardim, São Paulo - SP, CEP: 01234-567</t>
+  </si>
+  <si>
+    <t>João Davi</t>
+  </si>
+  <si>
+    <t>782.594.315-06</t>
+  </si>
+  <si>
+    <t>joao.silva23@hotmail.com</t>
+  </si>
+  <si>
+    <t>(21) 98765-4321</t>
+  </si>
+  <si>
+    <t>Avenida Atlântica, 456, Copacabana, Rio de Janeiro - RJ, CEP: 22070-001</t>
+  </si>
+  <si>
+    <t>Gustavão Gemeas</t>
+  </si>
+  <si>
+    <t>Renan Carlos</t>
+  </si>
+  <si>
+    <t>145.782.963-14</t>
+  </si>
+  <si>
+    <t>renan.alves99@outlook.com</t>
+  </si>
+  <si>
+    <t>(41) 99876-5432</t>
+  </si>
+  <si>
+    <t>Rua das Palmeiras, 100, Batel, Curitiba - PR, CEP: 80240-001</t>
+  </si>
+  <si>
+    <t>Trabalho</t>
+  </si>
+  <si>
+    <t>Trabalho.trabalhado@work.com</t>
+  </si>
+  <si>
+    <t>(99) 99999-9999</t>
+  </si>
+  <si>
+    <t>Rua Trabalho, 999, Trabai. CEP: 99999-9999</t>
+  </si>
+  <si>
+    <t>613.809.124-50</t>
+  </si>
+  <si>
+    <t>Luis Gustavo</t>
+  </si>
+  <si>
+    <t>gustavo.martins86@yahoo.com.br</t>
+  </si>
+  <si>
+    <t>(31) 98712-3456</t>
+  </si>
+  <si>
+    <t>Rua Afonso Pena, 789, Centro, Belo Horizonte - MG, CEP: 30130-907</t>
+  </si>
+  <si>
+    <t>fasfas</t>
+  </si>
+  <si>
+    <t>frwef</t>
+  </si>
+  <si>
+    <t>23131</t>
+  </si>
+  <si>
+    <t>fsdf</t>
+  </si>
+  <si>
+    <t>dasd</t>
+  </si>
+  <si>
+    <t>dsad</t>
+  </si>
+  <si>
+    <t>dsadas</t>
+  </si>
+  <si>
+    <t>das</t>
   </si>
 </sst>
 </file>
@@ -167,7 +290,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -192,70 +315,87 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>19</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>24</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>29</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>27</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>